<commit_message>
added utils script for function mgmt + created routines import
</commit_message>
<xml_diff>
--- a/data/liftingexceldoc.xlsx
+++ b/data/liftingexceldoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boydk\Desktop\Personal Lifting Project\py-project-directory\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC83999D-20DE-428E-BB3D-0E0D5AE5F74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C05C27-5075-412D-BC1B-78C6796D67C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{8B3EE465-2883-4BE7-9439-FC93EB33E87B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="9" xr2:uid="{8B3EE465-2883-4BE7-9439-FC93EB33E87B}"/>
   </bookViews>
   <sheets>
     <sheet name="Macrocycle" sheetId="3" r:id="rId1"/>
@@ -2836,17 +2836,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F81FDCF-BDF5-4709-B81D-7793554E6848}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24" style="20" bestFit="1" customWidth="1"/>
   </cols>
@@ -6212,7 +6210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6486572-3031-4711-8E4A-D6D5766FDAF2}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
corrected headers + added replace and append logic to weights import
</commit_message>
<xml_diff>
--- a/data/liftingexceldoc.xlsx
+++ b/data/liftingexceldoc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boydk\Desktop\Personal Lifting Project\py-project-directory\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16B9CCC-550E-4175-9FD8-30BD5DB29C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DB3D38-4EFE-4D2E-A1F0-0EF43AED41C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8B3EE465-2883-4BE7-9439-FC93EB33E87B}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="208">
   <si>
     <t>Mesocycle 1</t>
   </si>
@@ -677,9 +677,6 @@
   <si>
     <t>Off Day</t>
   </si>
-  <si>
-    <t>Day</t>
-  </si>
 </sst>
 </file>
 
@@ -6538,8 +6535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6486572-3031-4711-8E4A-D6D5766FDAF2}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6552,7 +6549,7 @@
         <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>